<commit_message>
updating amazon web scraping
</commit_message>
<xml_diff>
--- a/WebScraping_from_Amazon/product.xlsx
+++ b/WebScraping_from_Amazon/product.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Anchit Julaniya\Desktop\Assignments Geekster\Backend\WebScraping_from_Amazon\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA110AB-A1DF-41EA-B923-52827D097092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8251E7-41AB-41AA-9E54-752431D95C11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,6 +17,140 @@
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUKITEL WP36 2024 Rugged Smartphone - 10600mAh Rugged Phone 128dB Loud Speaker, 16GB+128GB Dual Sim Phones 6.52" Big Screen, Android 13 Cell Phone, NFC/OTG, T-mobile Compatible Rugged Smart Phone  </t>
+  </si>
+  <si>
+    <t>199.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4.4 out of 5 stars </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcatel 1 (32GB) 5.0" Full View Display - Removable Battery - Dual SIM GSM Unlocked US &amp; Global 4G LTE International Version - Al Aqua  </t>
+  </si>
+  <si>
+    <t>35.</t>
+  </si>
+  <si>
+    <t>4.4 out of 5 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total by Verizon TCL 30 Z, 32GB, Black - Prepaid Smartphone (Locked)  </t>
+  </si>
+  <si>
+    <t>39.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BLU G73 | 2023 | 3-Day Battery | Unlocked | 6.8” HD+ Infinity Display | 128/6GB | Triple 50MP Camera | US Version | US Warranty | Grey  </t>
+  </si>
+  <si>
+    <t>99.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung Galaxy A15 5G (SM-156M/DSN), 256GB 8GB RAM, Dual SIM, Factory Unlocked GSM, International Version (Wall Charger Bundle) (Light Blue)  </t>
+  </si>
+  <si>
+    <t>179.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG Galaxy A25 5G A Series Cell Phone, 128GB Unlocked Android Smartphone, AMOLED Display, Advanced Triple Camera System, Expandable Storage, Power Sound w/Stereo Speakers, US Version, 2024, Black  </t>
+  </si>
+  <si>
+    <t>300.</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nokia G100 | Verizon, T-Mobile, AT&amp;T | Android 12 | Unlocked Smartphone | 3-Day Battery | US Version | 4/128GB | 6.52-Inch Screen | 13MP Triple Camera | Polar Night  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.6 out of 5 stars </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG Galaxy A05s (128GB, 4GB) 6.7" Dual SIM GSM Unlocked Global 4G LTE A057M/DS (Black)  </t>
+  </si>
+  <si>
+    <t>119.</t>
+  </si>
+  <si>
+    <t>3.6 out of 5 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMSUNG Galaxy A35 5G A Series Cell Phone, 128GB Unlocked Android Smartphone, AMOLED Display, Advanced Triple Camera System, Expandable Storage, Rugged Design, US Version, 2024, Awesome Lilac  </t>
+  </si>
+  <si>
+    <t>359.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alcatel 1 (32GB) 5.0" Full View Display - Removable Battery - Dual SIM GSM Unlocked US &amp; Global 4G LTE International Version - Volcano Black  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">44  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panasonic Compact Cordless Phone with DECT 6.0, 1.6" Amber LCD and Illuminated HS Keypad, Call Block, Caller ID, Multiple Display Languages - 1 Handset - KX-TGB810S (Black/Silver)  </t>
+  </si>
+  <si>
+    <t>15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AT&amp;T 210 Basic Trimline Corded Phone, No AC Power Required, Wall-Mountable, White  </t>
+  </si>
+  <si>
+    <t>49.</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TracFone Samsung Galaxy A03s, 32GB, Black - Prepaid Smartphone (Locked)  </t>
+  </si>
+  <si>
+    <t>139.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3.9 out of 5 stars </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Samsung Galaxy A15 (SM-155M/DSN), 128GB 6GB RAM, Dual SIM, Factory Unlocked GSM, International Version (Ring Grip Case Bundle) (Light Blue)  </t>
+  </si>
+  <si>
+    <t>569.</t>
+  </si>
+  <si>
+    <t>3.9 out of 5 stars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8849 Tank 3 Rugged Smartphone, 23800mAh 5G Outdoor Rugged Cell Phone Unlocked, 32GB RAM+512GB ROM, 6.79" Waterproof Android 13 Mobile Phones, 200MP Main Camera/OTG/NFC(Support T-Mobile &amp; Verizon Only)  </t>
+  </si>
+  <si>
+    <t>52.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cheap Smartphone， 5.0'' Android 9.0, 16GB ROM(Extendable to 128GB,Dual SIM Dual Camera, WiFi,Bluetooth,GPS Basic Mobile Phones (R10-Purple)  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">26  </t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -391,15 +525,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.45"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>40</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="15.9" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:C17" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>